<commit_message>
Create conversion files and organize structures
</commit_message>
<xml_diff>
--- a/borehole_data.xlsx
+++ b/borehole_data.xlsx
@@ -599,7 +599,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>黄土-</t>
+          <t>黄土</t>
         </is>
       </c>
       <c r="B5" s="3" t="n">
@@ -667,7 +667,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>黄土-</t>
+          <t>黄土</t>
         </is>
       </c>
       <c r="B7" s="3" t="n">
@@ -701,7 +701,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>粉砂-</t>
+          <t>粉砂</t>
         </is>
       </c>
       <c r="B8" s="3" t="n">
@@ -735,7 +735,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>黏土0</t>
+          <t>黏土</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
@@ -803,7 +803,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>粉砂-</t>
+          <t>粉砂</t>
         </is>
       </c>
       <c r="B11" s="3" t="n">
@@ -837,7 +837,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>砾石0</t>
+          <t>砾石</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
@@ -871,7 +871,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>页岩0</t>
+          <t>页岩</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
@@ -905,7 +905,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>粉土-</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="B14" s="3" t="n">
@@ -939,7 +939,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>黏土-</t>
+          <t>黏土</t>
         </is>
       </c>
       <c r="B15" s="3" t="n">
@@ -973,7 +973,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>泥岩0</t>
+          <t>泥岩</t>
         </is>
       </c>
       <c r="B16" s="2" t="n">
@@ -1007,7 +1007,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>砾石-</t>
+          <t>砾石</t>
         </is>
       </c>
       <c r="B17" s="3" t="n">
@@ -1041,7 +1041,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>页岩-</t>
+          <t>页岩</t>
         </is>
       </c>
       <c r="B18" s="3" t="n">

</xml_diff>